<commit_message>
LAP22G87-73 #Bug fix Test [Implementation]
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment.xlsx
+++ b/LAPR3-2021-Self-Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bftv\Documents\lapr3-2021-g087\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D49D3D5-2DDC-4217-B25D-5B81EFBC9013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6040C474-4A1D-4FC7-B3BE-324060FD293F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="173">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>The students  have exceeded expectations </t>
-  </si>
-  <si>
-    <t>US111</t>
-  </si>
-  <si>
-    <t>US112</t>
   </si>
   <si>
     <t>Code Quality based on Sonarqube Data</t>
@@ -550,34 +544,64 @@
     <t>LAPR3 Project Group and Self-assessment v1.0</t>
   </si>
   <si>
-    <t>US201</t>
-  </si>
-  <si>
-    <t>US202</t>
-  </si>
-  <si>
-    <t>US203</t>
-  </si>
-  <si>
-    <t>US204</t>
-  </si>
-  <si>
-    <t>US205</t>
-  </si>
-  <si>
-    <t>US206</t>
-  </si>
-  <si>
-    <t>US207</t>
-  </si>
-  <si>
-    <t>US208</t>
-  </si>
-  <si>
-    <t>US209</t>
-  </si>
-  <si>
-    <t>US210</t>
+    <t>US301</t>
+  </si>
+  <si>
+    <t>US302</t>
+  </si>
+  <si>
+    <t>US303</t>
+  </si>
+  <si>
+    <t>US304</t>
+  </si>
+  <si>
+    <t>US305</t>
+  </si>
+  <si>
+    <t>US306</t>
+  </si>
+  <si>
+    <t>US307</t>
+  </si>
+  <si>
+    <t>US308</t>
+  </si>
+  <si>
+    <t>US309</t>
+  </si>
+  <si>
+    <t>US310</t>
+  </si>
+  <si>
+    <t>US311</t>
+  </si>
+  <si>
+    <t>US312</t>
+  </si>
+  <si>
+    <t>US313</t>
+  </si>
+  <si>
+    <t>US314</t>
+  </si>
+  <si>
+    <t>US315</t>
+  </si>
+  <si>
+    <t>US316</t>
+  </si>
+  <si>
+    <t>US317</t>
+  </si>
+  <si>
+    <t>US318</t>
+  </si>
+  <si>
+    <t>US319</t>
+  </si>
+  <si>
+    <t>US320</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1356,6 +1380,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2082,8 +2109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51149F-37F8-9041-812D-F0949B9CB00F}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2123,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2130,24 +2157,24 @@
     <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="79"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="79"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="80"/>
+      <c r="T8" s="81"/>
     </row>
     <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
@@ -2217,7 +2244,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="40">
@@ -2233,7 +2260,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
@@ -2248,11 +2275,11 @@
       <c r="R10" s="40"/>
       <c r="S10" s="53">
         <f>AVERAGE(D10:R10)</f>
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="76"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="8">
         <v>1200587</v>
       </c>
@@ -2266,7 +2293,7 @@
         <v>5</v>
       </c>
       <c r="G11" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -2281,11 +2308,11 @@
       <c r="R11" s="10"/>
       <c r="S11" s="54">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="76"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="8">
         <v>1192221</v>
       </c>
@@ -2299,7 +2326,7 @@
         <v>5</v>
       </c>
       <c r="G12" s="38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -2314,11 +2341,11 @@
       <c r="R12" s="10"/>
       <c r="S12" s="54">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="76"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="8">
         <v>1181122</v>
       </c>
@@ -2351,7 +2378,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="76"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="8" t="s">
         <v>7</v>
       </c>
@@ -2376,7 +2403,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="76"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="8" t="s">
         <v>8</v>
       </c>
@@ -2401,7 +2428,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="76"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
@@ -2426,7 +2453,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="76"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
@@ -2451,7 +2478,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="76"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="8" t="s">
         <v>11</v>
       </c>
@@ -2476,7 +2503,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="76"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="8" t="s">
         <v>12</v>
       </c>
@@ -2501,7 +2528,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="76"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="8" t="s">
         <v>13</v>
       </c>
@@ -2526,7 +2553,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="76"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="8" t="s">
         <v>14</v>
       </c>
@@ -2551,7 +2578,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="76"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="8" t="s">
         <v>15</v>
       </c>
@@ -2576,7 +2603,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="76"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="8" t="s">
         <v>16</v>
       </c>
@@ -2601,7 +2628,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="77"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="43" t="s">
         <v>17</v>
       </c>
@@ -2644,7 +2671,7 @@
       </c>
       <c r="G25" s="49">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="H25" s="49" t="e">
         <f t="shared" si="1"/>
@@ -2779,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2798,16 +2825,16 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="82" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="11">
@@ -2830,10 +2857,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="82"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="15" t="s">
         <v>33</v>
       </c>
@@ -2854,10 +2881,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="82"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="23" t="s">
         <v>39</v>
       </c>
@@ -2879,7 +2906,7 @@
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="8">
         <v>1192221</v>
@@ -2911,7 +2938,7 @@
     </row>
     <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B7" s="8">
         <v>1200587</v>
@@ -2943,10 +2970,10 @@
     </row>
     <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1191938</v>
+        <v>155</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1181122</v>
       </c>
       <c r="C8" s="8">
         <v>4</v>
@@ -2975,17 +3002,15 @@
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" s="8">
-        <v>1200587</v>
+        <v>1191938</v>
       </c>
       <c r="C9" s="8">
         <v>4</v>
       </c>
-      <c r="D9" s="13">
-        <v>1191938</v>
-      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="15" t="s">
         <v>39</v>
       </c>
@@ -3007,7 +3032,7 @@
     </row>
     <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B10" s="8">
         <v>1191938</v>
@@ -3039,17 +3064,15 @@
     </row>
     <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B11" s="8">
-        <v>1200587</v>
+        <v>1191938</v>
       </c>
       <c r="C11" s="8">
         <v>4</v>
       </c>
-      <c r="D11" s="13">
-        <v>1191938</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="15" t="s">
         <v>39</v>
       </c>
@@ -3071,7 +3094,7 @@
     </row>
     <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B12" s="8">
         <v>1200587</v>
@@ -3103,7 +3126,7 @@
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B13" s="8">
         <v>1191938</v>
@@ -3135,7 +3158,7 @@
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="8">
         <v>1191938</v>
@@ -3167,17 +3190,15 @@
     </row>
     <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1191938</v>
+        <v>162</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1200587</v>
       </c>
       <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1200587</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="15" t="s">
         <v>39</v>
       </c>
@@ -3199,7 +3220,7 @@
     </row>
     <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3225,10 +3246,14 @@
     </row>
     <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+        <v>164</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1200587</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4</v>
+      </c>
       <c r="D17" s="13"/>
       <c r="E17" s="15" t="s">
         <v>39</v>
@@ -3250,10 +3275,16 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="16"/>
+      <c r="A18" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1192221</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="13">
+        <v>1181122</v>
+      </c>
       <c r="E18" s="15" t="s">
         <v>39</v>
       </c>
@@ -3274,10 +3305,16 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1192221</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="13">
+        <v>1181122</v>
+      </c>
       <c r="E19" s="15" t="s">
         <v>39</v>
       </c>
@@ -3298,10 +3335,14 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1192221</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="15" t="s">
         <v>39</v>
       </c>
@@ -3322,10 +3363,14 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="16"/>
+      <c r="A21" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1181122</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="15" t="s">
         <v>39</v>
       </c>
@@ -3346,10 +3391,16 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="16"/>
+      <c r="A22" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1200587</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4</v>
+      </c>
+      <c r="D22" s="13"/>
       <c r="E22" s="15" t="s">
         <v>39</v>
       </c>
@@ -3370,10 +3421,16 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1200587</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4</v>
+      </c>
+      <c r="D23" s="13"/>
       <c r="E23" s="15" t="s">
         <v>39</v>
       </c>
@@ -3394,10 +3451,16 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="13">
+        <v>1200587</v>
+      </c>
+      <c r="C24" s="8">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="15" t="s">
         <v>39</v>
       </c>
@@ -3418,10 +3481,16 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="13">
+        <v>1200587</v>
+      </c>
+      <c r="C25" s="8">
+        <v>4</v>
+      </c>
+      <c r="D25" s="13"/>
       <c r="E25" s="23" t="s">
         <v>39</v>
       </c>
@@ -3448,6 +3517,7 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="E6">
     <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
       <formula>$C6=E$3</formula>
@@ -3533,11 +3603,8 @@
       <formula>$C7=J$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25" xr:uid="{81F67E9C-AEB8-4240-A844-E8F88E9A36EA}">
-      <formula1>$E$40:$J$40</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17" xr:uid="{69C19197-FA69-AA49-88F5-04A3AEDBB970}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C25" xr:uid="{69C19197-FA69-AA49-88F5-04A3AEDBB970}">
       <formula1>$E$3:$J$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3549,7 +3616,7 @@
           <x14:formula1>
             <xm:f>'Group and Self Assessment'!$C$10:$C$24</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B25</xm:sqref>
+          <xm:sqref>D15 B16:B20 B6:B7 B9:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3573,33 +3640,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="D3" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="E3" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="F3" s="58" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11">
         <v>34</v>
@@ -3620,7 +3687,7 @@
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="15">
         <v>21</v>
@@ -3641,7 +3708,7 @@
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="15">
         <v>-13</v>
@@ -3662,7 +3729,7 @@
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="23">
         <v>-13</v>
@@ -3683,7 +3750,7 @@
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="57">
         <v>55</v>
@@ -3702,7 +3769,7 @@
       <c r="C9" s="67"/>
       <c r="D9" s="68"/>
       <c r="E9" s="48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" s="69">
         <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
@@ -3720,7 +3787,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3742,7 +3809,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3762,10 +3829,10 @@
     <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -3855,7 +3922,7 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>32</v>
@@ -3863,7 +3930,7 @@
     </row>
     <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="18">
         <v>0.35</v>
@@ -3933,29 +4000,29 @@
         <v>2.938181818181818</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="18">
         <v>7.4999999999999997E-2</v>
@@ -3988,29 +4055,29 @@
         <v>5</v>
       </c>
       <c r="S5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="U5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="V5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="W5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="X5" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="18">
         <v>0.1</v>
@@ -4043,44 +4110,44 @@
         <v>4</v>
       </c>
       <c r="S6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="V6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="W6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="X6" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="18">
         <v>0.35</v>
       </c>
       <c r="C7" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
@@ -4095,32 +4162,32 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="28">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="U7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="V7" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="U7" s="7" t="s">
+      <c r="W7" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="V7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="X7" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" s="18">
         <v>0.125</v>
@@ -4145,29 +4212,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U8" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="T8" s="7" t="s">
+      <c r="V8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="U8" s="7" t="s">
+      <c r="W8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="V8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="X8" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="19">
         <f>SUM(B4:B8)</f>
@@ -4175,19 +4242,19 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>3.2033636363636364</v>
+        <v>2.8533636363636363</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>3.2033636363636364</v>
+        <v>2.8533636363636363</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>3.2033636363636364</v>
+        <v>2.8533636363636363</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>3.2033636363636364</v>
+        <v>2.8533636363636363</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
@@ -4245,24 +4312,24 @@
     </row>
     <row r="10" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>12.813454545454546</v>
+        <v>11.413454545454545</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>12.813454545454546</v>
+        <v>11.413454545454545</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="2"/>
-        <v>12.813454545454546</v>
+        <v>11.413454545454545</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>12.813454545454546</v>
+        <v>11.413454545454545</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
@@ -4320,7 +4387,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -4338,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C190218-096C-D04F-B5E6-6BE0B32B2632}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4359,7 +4426,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="14"/>
@@ -4378,10 +4445,10 @@
     </row>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -4471,7 +4538,7 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>32</v>
@@ -4479,7 +4546,7 @@
     </row>
     <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="18">
         <v>0.1</v>
@@ -4512,29 +4579,29 @@
         <v>4</v>
       </c>
       <c r="S4" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="U4" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="T4" s="74" t="s">
+      <c r="V4" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="U4" s="74" t="s">
+      <c r="W4" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="V4" s="74" t="s">
+      <c r="X4" s="74" t="s">
         <v>98</v>
-      </c>
-      <c r="W4" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="X4" s="74" t="s">
-        <v>100</v>
       </c>
       <c r="Y4" s="71"/>
       <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="18">
         <v>0.1</v>
@@ -4567,29 +4634,29 @@
         <v>4</v>
       </c>
       <c r="S5" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="T5" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="T5" s="74" t="s">
+      <c r="V5" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="U5" s="74" t="s">
+      <c r="W5" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="V5" s="74" t="s">
+      <c r="X5" s="74" t="s">
         <v>105</v>
-      </c>
-      <c r="W5" s="74" t="s">
-        <v>106</v>
-      </c>
-      <c r="X5" s="74" t="s">
-        <v>107</v>
       </c>
       <c r="Y5" s="71"/>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" s="18">
         <v>0.05</v>
@@ -4622,44 +4689,44 @@
         <v>5</v>
       </c>
       <c r="S6" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="T6" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="U6" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="74" t="s">
+      <c r="V6" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="U6" s="74" t="s">
+      <c r="W6" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="V6" s="74" t="s">
+      <c r="X6" s="74" t="s">
         <v>112</v>
-      </c>
-      <c r="W6" s="74" t="s">
-        <v>113</v>
-      </c>
-      <c r="X6" s="74" t="s">
-        <v>114</v>
       </c>
       <c r="Y6" s="71"/>
       <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" s="18">
         <v>0.05</v>
       </c>
       <c r="C7" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
@@ -4674,32 +4741,32 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="70">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S7" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="T7" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="U7" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="V7" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="U7" s="74" t="s">
+      <c r="W7" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="V7" s="74" t="s">
+      <c r="X7" s="74" t="s">
         <v>118</v>
-      </c>
-      <c r="W7" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="X7" s="74" t="s">
-        <v>120</v>
       </c>
       <c r="Y7" s="71"/>
       <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" s="18">
         <v>0.1</v>
@@ -4732,29 +4799,29 @@
         <v>4</v>
       </c>
       <c r="S8" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="T8" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="U8" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="V8" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="U8" s="74" t="s">
+      <c r="W8" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="V8" s="74" t="s">
+      <c r="X8" s="74" t="s">
         <v>124</v>
-      </c>
-      <c r="W8" s="74" t="s">
-        <v>125</v>
-      </c>
-      <c r="X8" s="74" t="s">
-        <v>126</v>
       </c>
       <c r="Y8" s="71"/>
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B9" s="18">
         <v>0.05</v>
@@ -4787,25 +4854,25 @@
         <v>3</v>
       </c>
       <c r="S9" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T9" s="74" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U9" s="74"/>
       <c r="V9" s="74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="W9" s="74"/>
       <c r="X9" s="74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y9" s="71"/>
       <c r="Z9" s="16"/>
     </row>
     <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B10" s="18">
         <v>0.1</v>
@@ -4838,29 +4905,29 @@
         <v>3</v>
       </c>
       <c r="S10" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T10" s="74" t="s">
+        <v>131</v>
+      </c>
+      <c r="U10" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="V10" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="U10" s="74" t="s">
+      <c r="W10" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="V10" s="74" t="s">
+      <c r="X10" s="74" t="s">
         <v>135</v>
-      </c>
-      <c r="W10" s="74" t="s">
-        <v>136</v>
-      </c>
-      <c r="X10" s="74" t="s">
-        <v>137</v>
       </c>
       <c r="Y10" s="71"/>
       <c r="Z10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B11" s="18">
         <v>0.1</v>
@@ -4893,29 +4960,29 @@
         <v>2</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T11" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="U11" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="V11" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="U11" s="74" t="s">
+      <c r="W11" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="V11" s="74" t="s">
+      <c r="X11" s="74" t="s">
         <v>141</v>
-      </c>
-      <c r="W11" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="X11" s="74" t="s">
-        <v>143</v>
       </c>
       <c r="Y11" s="71"/>
       <c r="Z11" s="16"/>
     </row>
     <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12" s="18">
         <v>0.1</v>
@@ -4940,29 +5007,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T12" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="U12" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="V12" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="U12" s="74" t="s">
+      <c r="W12" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="V12" s="74" t="s">
+      <c r="X12" s="74" t="s">
         <v>141</v>
-      </c>
-      <c r="W12" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="X12" s="74" t="s">
-        <v>143</v>
       </c>
       <c r="Y12" s="71"/>
       <c r="Z12" s="16"/>
     </row>
     <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="18">
         <v>0.1</v>
@@ -4987,29 +5054,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S13" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="T13" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="U13" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="T13" s="74" t="s">
+      <c r="V13" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="U13" s="74" t="s">
+      <c r="W13" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="V13" s="74" t="s">
+      <c r="X13" s="74" t="s">
         <v>149</v>
-      </c>
-      <c r="W13" s="74" t="s">
-        <v>150</v>
-      </c>
-      <c r="X13" s="74" t="s">
-        <v>151</v>
       </c>
       <c r="Y13" s="71"/>
       <c r="Z13" s="16"/>
     </row>
     <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B14" s="18">
         <v>0.15</v>
@@ -5034,29 +5101,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T14" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="U14" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="V14" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="U14" s="74" t="s">
+      <c r="W14" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="V14" s="74" t="s">
+      <c r="X14" s="74" t="s">
         <v>141</v>
-      </c>
-      <c r="W14" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="X14" s="74" t="s">
-        <v>143</v>
       </c>
       <c r="Y14" s="71"/>
       <c r="Z14" s="16"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="19">
         <f>SUM(B4:B14)</f>
@@ -5134,7 +5201,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24">
@@ -5209,7 +5276,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -5236,21 +5303,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -5434,31 +5486,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5474,4 +5517,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>